<commit_message>
Update for the release.
Signed-off-by: Keshava Munegowda <keshava.gowda@gmail.com>
</commit_message>
<xml_diff>
--- a/samples/charts/sbk-file-rocksdb-read.xlsx
+++ b/samples/charts/sbk-file-rocksdb-read.xlsx
@@ -85,7 +85,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="16">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -129,6 +129,38 @@
       <color rgb="FF008000"/>
       <sz val="18"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FFFF0000"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FF0000"/>
+      <sz val="18"/>
+    </font>
+    <font>
+      <color rgb="0000CF00"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00EE00FF"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <color rgb="FF800000"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="0000AA00"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <color rgb="FF000080"/>
+      <sz val="14"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -138,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -146,11 +178,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -175,6 +213,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9200,7 +9251,7 @@
           <idx val="0"/>
           <order val="0"/>
           <tx>
-            <v>T1_FILE_2</v>
+            <v>T1_FILE_1</v>
           </tx>
           <spPr>
             <a:ln>
@@ -9230,7 +9281,7 @@
           <idx val="1"/>
           <order val="1"/>
           <tx>
-            <v>T2_ROCKSDB_2</v>
+            <v>T2_ROCKSDB_1</v>
           </tx>
           <spPr>
             <a:ln>
@@ -9343,7 +9394,7 @@
           <idx val="0"/>
           <order val="0"/>
           <tx>
-            <v>T1_FILE_2</v>
+            <v>T1_FILE_1</v>
           </tx>
           <spPr>
             <a:ln>
@@ -9373,7 +9424,7 @@
           <idx val="1"/>
           <order val="1"/>
           <tx>
-            <v>T2_ROCKSDB_2</v>
+            <v>T2_ROCKSDB_1</v>
           </tx>
           <spPr>
             <a:ln>
@@ -9487,7 +9538,7 @@
           <idx val="0"/>
           <order val="0"/>
           <tx>
-            <v>T1_FILE_2</v>
+            <v>T1_FILE_1</v>
           </tx>
           <spPr>
             <a:ln>
@@ -9509,7 +9560,7 @@
           <idx val="1"/>
           <order val="1"/>
           <tx>
-            <v>T2_ROCKSDB_2</v>
+            <v>T2_ROCKSDB_1</v>
           </tx>
           <spPr>
             <a:ln>
@@ -33136,7 +33187,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="G7:H15"/>
+  <dimension ref="G7:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33145,7 +33196,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="45" customWidth="1" min="7" max="7"/>
-    <col width="75" customWidth="1" min="8" max="8"/>
+    <col width="108" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="7">
@@ -33163,7 +33214,7 @@
       </c>
       <c r="H8" s="3" t="inlineStr">
         <is>
-          <t>1.25.12.0</t>
+          <t>2.25.12.0</t>
         </is>
       </c>
     </row>
@@ -33174,7 +33225,7 @@
         </is>
       </c>
       <c r="H9" s="5" t="n">
-        <v>46009</v>
+        <v>46019</v>
       </c>
     </row>
     <row r="10">
@@ -33185,7 +33236,7 @@
       </c>
       <c r="H10" s="6" t="inlineStr">
         <is>
-          <t>19:25:04</t>
+          <t>17:24:19</t>
         </is>
       </c>
     </row>
@@ -33217,6 +33268,83 @@
       <c r="H15" s="11" t="inlineStr">
         <is>
           <t>FILE, ROCKSDB</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="70" customHeight="1">
+      <c r="H18" s="12" t="inlineStr">
+        <is>
+          <t>The AI may hallucinate !. The summary generated by generative AI models may not be complete and accurate. It's recommended to analyze the graphs along with the generated summary.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="G20" s="13" t="inlineStr">
+        <is>
+          <t>AI Performance Analysis</t>
+        </is>
+      </c>
+      <c r="H20" s="14" t="inlineStr">
+        <is>
+          <t>Hugging Face Inference APIs with model ID: google/gemma-2-2b-it</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="600" customHeight="1">
+      <c r="G22" s="15" t="inlineStr">
+        <is>
+          <t>Throughput Analysis</t>
+        </is>
+      </c>
+      <c r="H22" s="16" t="inlineStr">
+        <is>
+          <t>Let's break down the storage throughput performance analysis.
+**Throughput Analysis**
+* **FILE System:** The FILE system demonstrates a clear performance advantage, achieving an average throughput of 19.60 MB/s.  The minimum throughput recorded is 18.91 MB/s, while the maximum reaches 19.74 MB/s. This indicates a relatively consistent performance with a small variance. 
+* **ROCKSDB System:** The ROCKSDB system shows significantly lower throughput, with an average of 7.91 MB/s.  The minimum throughput is a modest 2.14 MB/s, while the maximum reaches 8.82 MB/s. This suggests a considerable gap in performance compared to the FILE system. 
+**Relative Performance Differences**
+The FILE system exhibits a roughly **2x** higher throughput compared to the ROCKSDB system.
+**Observations and Insights**
+The significant performance difference between the FILE system and the ROCKSDB system suggests that the FILE system is more suited for high-throughput workloads. The FILE system's performance is consistent across different data access patterns, while the ROCKSDB system's performance fluctuates more.  
+**Further Considerations:**
+* **Workload Characteristics:** The specific workload characteristics, including data access patterns, workload characteristics, and database configuration, will significantly impact performance. 
+* **System Configuration:**  Hardware configurations, including storage devices, network infrastructure, and system utilization, can impact overall throughput. 
+* **Data Distribution:** The distribution of data across the storage system can also influence performance. 
+* **Benchmarking Methodology:** The benchmarking methodology used, including the number of reads/writes performed, time duration, and data size, can impact the results.  
+To gain a deeper understanding of the differences, further investigation into the specific configuration of the systems, as well as benchmarking under similar workloads, is necessary.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="1000" customHeight="1">
+      <c r="G23" s="17" t="inlineStr">
+        <is>
+          <t>Latency Analysis</t>
+        </is>
+      </c>
+      <c r="H23" s="18" t="inlineStr">
+        <is>
+          <t>## Storage System Latency Analysis
+This analysis examines latency metrics across two storage systems: FILE and ROCKSDB. 
+**1. Comparison of Latency Profiles and Total Records:**
+The FILE system exhibits significantly higher latency than the ROCKSDB system, particularly for reading operations. This is reflected in the average latency (437.90 ns vs. 1159.40 ns), median latency (417.00 ns vs. 1041.00 ns), and 95th percentile latency (541.00 ns vs. 1375.00 ns). This difference suggests that FILE is likely to have a slower response time for read operations, potentially impacting application performance. 
+The total number of records processed by each system is also notable. FILE processes a significantly larger number of records (246,578,839) compared to ROCKSDB (99,485,873). This higher volume could influence the latency observed in the system.
+**2. Percentiles for Different Storage Systems:**
+* **FILE:** The p99.9 latency for FILE is 834.00 ns, indicating that 99.9% of read requests take longer than this. 
+* **ROCKSDB:** The p99.9 latency for ROCKSDB is 8417.00 ns, suggesting that a much smaller proportion of read requests exceed this threshold.
+This difference in p99.9 latency points to the potential for different levels of responsiveness depending on the specific workload.
+**3. Impact of Total Records and Time Unit:**
+The total number of records processed significantly influences the observed latency. The larger dataset handled by FILE contributes to its higher average and tail latencies. This emphasizes the importance of balancing throughput and latency requirements when choosing a storage system. 
+The time unit used in the data also impacts interpretation. While the difference in latency is significant, it's important to consider that the data represents nanosecond-level latency, which is extremely fast. 
+**4.  Significant Differences and Anomalies:**
+The significant difference in latency between FILE and ROCKSDB is indicative of a performance trade-off. While FILE's high average latency might be acceptable for certain workloads, its p99.9 latency suggests potential performance bottlenecks in specific scenarios. 
+Further investigation into the specific workload characteristics and configuration of both systems is needed to determine the root cause of these performance differences and optimize each system for its respective use case.
+**5. Implications for Storage Engineers:**
+Based on these findings, storage engineers should consider the following:
+* **Performance Optimization:** Investigate potential optimizations for the FILE system, such as tuning its configuration parameters or utilizing load balancing techniques.
+* **Workload Compatibility:** Evaluate the suitability of each system for the specific workload requirements, considering both average latency and tail latency.
+* **Monitoring and Alerting:** Implement monitoring mechanisms to track system performance and alert engineers in case of any significant latency spikes or anomalies.
+* **Resource Allocation:** Allocate resources strategically to ensure optimal performance for each system based on its specific characteristics. 
+By understanding these nuances, storage engineers can make informed decisions to optimize system performance and ensure reliable data storage and retrieval.</t>
         </is>
       </c>
     </row>

</xml_diff>